<commit_message>
precisiones y adiciones en analisis de datos
</commit_message>
<xml_diff>
--- a/docs/trim1/2_levantamiento_informacion/1_recoleccion_informacion.xlsx
+++ b/docs/trim1/2_levantamiento_informacion/1_recoleccion_informacion.xlsx
@@ -20,7 +20,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Hoja de Control'!$B$2:$F$44</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">Instrumentos!$A$1:$K$119</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">Planeación!$A$1:$J$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area" vbProcedure="false">Tabulación!$A$1:$K$116</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area" vbProcedure="false">Tabulación!$A$1:$K$115</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area" vbProcedure="false">Técnicas!$A$1:$K$116</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="96">
   <si>
     <t xml:space="preserve">Proyecto Inventario Miscelánea Ginna Marcela</t>
   </si>
@@ -194,7 +194,7 @@
     <t xml:space="preserve">Libreta de apuntes</t>
   </si>
   <si>
-    <t xml:space="preserve">Identificar reglamentaciones relacionadascon captura y recolección de datos para el sistema</t>
+    <t xml:space="preserve">Identificar reglamentaciones relacionadas con captura y recolección de datos para el sistema</t>
   </si>
   <si>
     <t xml:space="preserve">Investigación</t>
@@ -203,6 +203,9 @@
     <t xml:space="preserve">Internet</t>
   </si>
   <si>
+    <t xml:space="preserve">William Arias</t>
+  </si>
+  <si>
     <t xml:space="preserve">Técnicas de Recolección</t>
   </si>
   <si>
@@ -275,38 +278,122 @@
     <t xml:space="preserve">Algunos fragmentos clave extraídos de la entrevista son</t>
   </si>
   <si>
-    <t xml:space="preserve">● "He realizado varios emprendimientos en diferentes negocios [...]"
-● "Es un negocio de mucha rentabilidad, ya que se encuentra mucha variedad, alta demanda y un gran porcentaje de ganancia"
-● "el negocio lleva más o menos 12 años"
-● "se comercializan productos de uso diario [...] para el hogar, cuidado del cuerpo, papelería, juguetería y variedad de cosas [...]"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">● "La mayoría de proveedores van hasta mi negocio [..] otro porcentaje de proveedores, yo tengo que ir directamente hasta su punto de venta para realizar la compra"
-● "No realizo ningún registro en el negocio [...] Siento que esa es una falencia [...], por mis deberes no me alcanza el tiempo para tener presente qué es lo que tengo"
-● "No tengo una base exacta de mis ingresos o de mis gastos"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">● "No sabría decirlo, ya que siempre estoy reinvirtiendo las ganancias o el capital en más productos"
-● "el cliente viene, solicita lo que está buscando, yo le paso variedad de productos que tengo referente al producto que necesita, escoge el que más le gusta, yo le realizo la venta del producto que yo tengo y listo"
-● "Dependiendo del cliente yo le realizo factura. Si él lo solicita o si es para una empresa, normalmente las hago en un talonario de facturas y con mi sello propio"</t>
+    <t xml:space="preserve">1. "He realizado varios emprendimientos en diferentes negocios […]"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. "Es un negocio de mucha rentabilidad, ya que se encuentra mucha variedad, alta demanda y un gran porcentaje de ganancia"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. "el negocio lleva más o menos 12 años"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. "se comercializan productos de uso diario [...] para el hogar, cuidado del cuerpo, papelería, juguetería y variedad de cosas [...]"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. "La mayoría de proveedores van hasta mi negocio [..] otro porcentaje de proveedores, yo tengo que ir directamente hasta su punto de venta para realizar la compra"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. "No realizo ningún registro en el negocio [...] Siento que esa es una falencia [...], por mis deberes no me alcanza el tiempo para tener presente qué es lo que tengo"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. "No tengo una base exacta de mis ingresos o de mis gastos"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. "No sabría decirlo, ya que siempre estoy reinvirtiendo las ganancias o el capital en más productos"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. "el cliente viene, solicita lo que está buscando, yo le paso variedad de productos que tengo referente al producto que necesita, escoge el que más le gusta, yo le realizo la venta del producto que yo tengo y listo"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. "Dependiendo del cliente yo le realizo factura. Si él lo solicita o si es para una empresa, normalmente las hago en un talonario de facturas y con mi sello propio"</t>
   </si>
   <si>
     <t xml:space="preserve">Análisis de la Información</t>
   </si>
   <si>
-    <t xml:space="preserve">En las preguntas de contexto se evidencia experiencia de la dueña en el manejo de negocios de comercio, incluso del mismo sector comercial de papelería. Al respecto, ella manifiesta saber que la miscelánea es un buen negocio que deja rentabilidad. Tanto en la ubicación anterior como en la que se encuentra actualmente. Además, se mencionan cuatro categorías de los productos que comercializa el negocio: Hogar, Cuidado Personal, Papelería y Juguetería. Estas categorías pueden ser útiles para la posterior clasificación de los productos en el sistema.</t>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial1"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">En la respuesta a las preguntas de contexto se evidencia experiencia de la dueña en el manejo de negocios de comercio, incluso del mismo sector comercial de papelería. Como menciona en: “</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial2"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">He realizado varios emprendimientos en diferentes negocios […]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial1"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">” (véase la tabulación de la información, fragmento de contexto 1.).
+Al respecto, ella manifiesta saber que la miscelánea es un buen negocio que deja rentabilidad. Tanto en la ubicación anterior como en la que se encuentra actualmente. 
+“</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial2"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Es un negocio de mucha rentabilidad, ya que se encuentra mucha variedad, alta demanda y un gran porcentaje de ganancia"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial1"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (Fragmento contexto  2.)
+Además, se mencionan cuatro categorías de los productos que comercializa el negocio: Hogar, Cuidado Personal, Papelería y Juguetería. Estas categorías pueden ser útiles para la posterior clasificación de los productos en el sistema.
+“</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial2"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">se comercializan productos de uso diario [...] para el hogar, cuidado del cuerpo, papelería, juguetería y variedad de cosas […]” (Fragmento contexto 4.).</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">En el proceso de compra de productos, se describen dos tipos de proveedores: los que se desplazan hacia la miscelánea y los que la dueña debe visitar para abastecerse. Los doce proveedores que manifiesta tener se dividen en estos dos tipos. 
-Es importante resaltar que la dueña es conciente de que no mantener ningún registro de entrada y salida de los productos que comercializa es una falencia para el negocio. Además de que expresa directamente que no tiene una base exacta de los ingresos y los gastos de la miscelánea. Expresa que las ganancias son la cantidad de dinero en caja. Este punto representa una oportunidad clave para el desarrollo y la implementación del sistema MGM, puesto que pretende cubrir la necesidad de información.</t>
+“"La mayoría de proveedores van hasta mi negocio [..] otro porcentaje de proveedores, yo tengo que ir directamente hasta su punto de venta” (Fragmento compra 1.).
+Es importante resaltar que la dueña es consciente de que no mantener ningún registro de entrada y salida de los productos que comercializa es una falencia para el negocio. Además de que expresa directamente que no tiene una base exacta de los ingresos y los gastos de la miscelánea. 
+“No realizo ningún registro en el negocio [...] Siento que esa es una falencia [...], por mis deberes no me alcanza el tiempo” (Fragmento compra 2.).
+Expresa que las ganancias son la cantidad de dinero en caja. Este punto representa una oportunidad clave para el desarrollo y la implementación del sistema MGM, puesto que pretende cubrir la necesidad de información.
+“No tengo una base exacta de mis ingresos o de mis gastos" (Fragmento compra 3.).</t>
   </si>
   <si>
     <t xml:space="preserve">Es importante resaltar que la dueña es conciente de que no mantener ningún registro de entrada y salida de los productos que comercializa es una falencia para el negocio. Además de que expresa directamente que no tiene una base exacta de los ingresos y los gastos de la miscelánea. Expresa que las ganancias son la cantidad de dinero en caja. Este punto representa una oportunidad clave para el desarrollo y la implementación del sistema MGM, puesto que pretende cubrir la necesidad de información.</t>
   </si>
   <si>
-    <t xml:space="preserve">La miscelánea no realiza ninguna adición o modificación al producto que vende. Lo que ubica a la microempresa Ginna Marcela en el negocio de la reventa de productos, de esta manera, sus ingresos provienen de la cantidad adicional se le añade al precio del producto final. En esa vía, ante la pregunta sobre el promedio de ingresos mensuales a raíz de las ventas de la microempresa, la dueña desconoce una cifra aproximada, y expresa que siempre está reinvirtiendo las ganancias en más productos.   
-Nuevamente, el desconocimiento de información como los ingresos mensuales se convierte en una oportunidad para que el sistema MGM supla esta necesidad, ya que con cifras claras de ingresos, puede tomar decisiones de reinversión más efectivas.  
-Por otro lado, el proceso de venta finaliza con el producto en las manos del cliente. La transacción se hace en efectivo y finaliza sin factura, siempre y cuando esta no sea solicitada. La dueña expresa que si el cliente es empresa o si explicitamente solicita la factura ella registra la venta en un talonario y le pone su sello propio de la miscelánea. </t>
+    <t xml:space="preserve">La miscelánea no realiza ninguna adición o modificación al producto que vende. Lo que ubica a la microempresa Ginna Marcela en el negocio de la reventa de productos, de esta manera, sus ingresos provienen de la cantidad adicional que se le añade al precio del producto final. En esa vía, ante la pregunta sobre el promedio de ingresos mensuales a raíz de las ventas de la microempresa, la dueña desconoce una cifra aproximada, y expresa que siempre está reinvirtiendo las ganancias en más productos.   
+“No sabría decirlo, ya que siempre estoy reinvirtiendo las ganancias o el capital en más productos" (Fragmento venta 1.).
+Nuevamente, el desconocimiento de información como los ingresos mensuales se convierte en una oportunidad para que el sistema MGM supla esta necesidad, ya que con cifras claras de ingresos puede tomar decisiones de reinversión más efectivas.  
+Por otro lado, el proceso de venta finaliza con el producto en las manos del cliente. La transacción se hace en efectivo y finaliza sin factura, siempre y cuando esta no sea solicitada. La dueña expresa que si el cliente es empresa o si explicitamente solicita la factura ella registra la venta en un talonario y le pone su sello propio de la miscelánea. 
+“Dependiendo del cliente yo le realizo factura. Si él lo solicita o si es para una empresa, normalmente las hago en un talonario de facturas y con mi sello propio” (Fragmento venta 3.).
+Con estos detalles se puede evidenciar dos elementos que surgen como necesidades: la falencia en el registro de productos entrantes y salientes y la carencia de información financiera base para la reinversión en nuevos productos.  Esta información es clave en el funcionamiento de la microempresa, ya que, como se mencionó, su modelo de negocio se basa en la reventa, y con la información oportuna podrá hacer mejores reinversiones. Además, la dueña parece realizar las reinversiones periódicamente, lo que se vincula como característica al sistema a implementar, en la medida que el sistema de inventario, al final del período o cuando ella desea reinvertir, proporcione una base para la decidir qué comprar y qué no.</t>
   </si>
 </sst>
 </file>
@@ -318,7 +405,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="dd\-mmm\-yy"/>
   </numFmts>
-  <fonts count="32">
+  <fonts count="31">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -535,14 +622,9 @@
     <font>
       <sz val="14"/>
       <color rgb="FF000000"/>
-      <name val="Arial1"/>
+      <name val="Arial2"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial1"/>
-      <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1149,187 +1231,187 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="3" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="3" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="3" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="3" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="4" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="4" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="4" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="4" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="6" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="6" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="7" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="7" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="4" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="4" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="2" borderId="3" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="8" fillId="2" borderId="3" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="8" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="8" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="9" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="9" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="21" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="2" borderId="4" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="8" fillId="2" borderId="4" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="10" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="10" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="2" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="8" fillId="2" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="11" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="11" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="12" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="12" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="13" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="13" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="14" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="14" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="15" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="15" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="16" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="16" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="17" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="17" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="18" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="18" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="19" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="19" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="19" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="19" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="20" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="20" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="21" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="21" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="21" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="21" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="22" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="22" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="23" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="23" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="21" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="21" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="4" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="4" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1337,203 +1419,203 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="4" borderId="1" xfId="20" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="14" fillId="4" borderId="1" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="24" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="24" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="25" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="25" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="5" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="5" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="5" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="5" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="5" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="5" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="20" fillId="0" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="20" fillId="0" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="32" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="32" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="33" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="33" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="32" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="32" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="34" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="34" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="32" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="32" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="4" borderId="35" xfId="20" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="14" fillId="4" borderId="35" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="35" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="35" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="35" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="35" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="25" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="25" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="36" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="36" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="32" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="32" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="37" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="37" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="23" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="23" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="38" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="38" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="39" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="39" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="40" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="40" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="41" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="41" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="42" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="42" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="32" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="32" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="32" xfId="21" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="32" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="32" xfId="21" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="32" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="24" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="24" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="32" xfId="21" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="32" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="4" borderId="43" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="29" fillId="4" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="4" borderId="43" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="23" fillId="4" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="4" borderId="43" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="29" fillId="4" borderId="44" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="30" fillId="4" borderId="43" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="30" fillId="4" borderId="43" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1622,9 +1704,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1424520</xdr:colOff>
+      <xdr:colOff>1423800</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>52920</xdr:rowOff>
+      <xdr:rowOff>52200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1638,7 +1720,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1771560" y="819360"/>
-          <a:ext cx="719640" cy="719640"/>
+          <a:ext cx="718920" cy="718920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1664,9 +1746,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>498240</xdr:colOff>
+      <xdr:colOff>497520</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>174240</xdr:rowOff>
+      <xdr:rowOff>173520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1680,7 +1762,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="66600" y="419040"/>
-          <a:ext cx="431640" cy="431640"/>
+          <a:ext cx="430920" cy="430920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1706,9 +1788,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1263240</xdr:colOff>
+      <xdr:colOff>1262520</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>277920</xdr:rowOff>
+      <xdr:rowOff>277200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1722,7 +1804,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1430280" y="845280"/>
-          <a:ext cx="899640" cy="899640"/>
+          <a:ext cx="898920" cy="898920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1748,9 +1830,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1263240</xdr:colOff>
+      <xdr:colOff>1262520</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>277920</xdr:rowOff>
+      <xdr:rowOff>277200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1764,7 +1846,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1430280" y="845280"/>
-          <a:ext cx="899640" cy="899640"/>
+          <a:ext cx="898920" cy="898920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1790,9 +1872,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1263240</xdr:colOff>
+      <xdr:colOff>1262520</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>277920</xdr:rowOff>
+      <xdr:rowOff>277200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1806,7 +1888,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1430280" y="845280"/>
-          <a:ext cx="899640" cy="899640"/>
+          <a:ext cx="898920" cy="898920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1832,9 +1914,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1263240</xdr:colOff>
+      <xdr:colOff>1262520</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>277920</xdr:rowOff>
+      <xdr:rowOff>277200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1848,7 +1930,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1430280" y="845280"/>
-          <a:ext cx="899640" cy="899640"/>
+          <a:ext cx="898920" cy="898920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1864,7 +1946,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -2547,14 +2629,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A3:IS34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2726,7 +2808,7 @@
         <v>44976</v>
       </c>
       <c r="G12" s="61" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="H12" s="66"/>
       <c r="I12" s="67"/>
@@ -2900,7 +2982,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -2945,7 +3027,7 @@
     </row>
     <row r="8" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -2982,7 +3064,7 @@
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="75"/>
       <c r="B13" s="76" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C13" s="76"/>
       <c r="D13" s="76"/>
@@ -3218,7 +3300,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -3266,7 +3348,7 @@
     </row>
     <row r="8" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -3303,7 +3385,7 @@
     <row r="13" customFormat="false" ht="23.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="12"/>
       <c r="B13" s="85" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C13" s="85"/>
       <c r="D13" s="85"/>
@@ -3323,7 +3405,7 @@
     <row r="15" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="12"/>
       <c r="B15" s="87" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C15" s="87"/>
       <c r="D15" s="87"/>
@@ -3334,7 +3416,7 @@
     <row r="16" s="1" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="12"/>
       <c r="B16" s="88" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C16" s="88"/>
       <c r="D16" s="88"/>
@@ -3348,7 +3430,7 @@
     <row r="17" s="1" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="12"/>
       <c r="B17" s="88" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C17" s="88"/>
       <c r="D17" s="88"/>
@@ -3362,7 +3444,7 @@
     <row r="18" s="1" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="12"/>
       <c r="B18" s="88" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C18" s="88"/>
       <c r="D18" s="88"/>
@@ -3388,7 +3470,7 @@
     <row r="20" s="1" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="12"/>
       <c r="B20" s="87" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C20" s="87"/>
       <c r="D20" s="87"/>
@@ -3402,7 +3484,7 @@
     <row r="21" s="1" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="12"/>
       <c r="B21" s="88" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C21" s="88"/>
       <c r="D21" s="88"/>
@@ -3414,7 +3496,7 @@
     <row r="22" s="1" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="12"/>
       <c r="B22" s="88" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C22" s="88"/>
       <c r="D22" s="88"/>
@@ -3426,7 +3508,7 @@
     <row r="23" s="1" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="12"/>
       <c r="B23" s="88" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C23" s="88"/>
       <c r="D23" s="88"/>
@@ -3438,7 +3520,7 @@
     <row r="24" s="1" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="12"/>
       <c r="B24" s="88" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C24" s="88"/>
       <c r="D24" s="88"/>
@@ -3450,7 +3532,7 @@
     <row r="25" s="1" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="12"/>
       <c r="B25" s="88" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C25" s="88"/>
       <c r="D25" s="88"/>
@@ -3472,7 +3554,7 @@
     <row r="27" s="1" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="12"/>
       <c r="B27" s="87" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C27" s="87"/>
       <c r="D27" s="87"/>
@@ -3484,7 +3566,7 @@
     <row r="28" s="1" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="12"/>
       <c r="B28" s="88" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C28" s="88"/>
       <c r="D28" s="88"/>
@@ -3496,7 +3578,7 @@
     <row r="29" s="1" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="12"/>
       <c r="B29" s="88" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C29" s="88"/>
       <c r="D29" s="88"/>
@@ -3508,7 +3590,7 @@
     <row r="30" s="1" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="12"/>
       <c r="B30" s="88" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C30" s="88"/>
       <c r="D30" s="88"/>
@@ -3520,7 +3602,7 @@
     <row r="31" s="1" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="12"/>
       <c r="B31" s="88" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C31" s="88"/>
       <c r="D31" s="88"/>
@@ -3532,7 +3614,7 @@
     <row r="32" s="1" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="12"/>
       <c r="B32" s="88" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C32" s="88"/>
       <c r="D32" s="88"/>
@@ -3544,7 +3626,7 @@
     <row r="33" s="1" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="12"/>
       <c r="B33" s="88" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C33" s="88"/>
       <c r="D33" s="88"/>
@@ -3556,7 +3638,7 @@
     <row r="34" s="1" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="12"/>
       <c r="B34" s="88" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C34" s="88"/>
       <c r="D34" s="88"/>
@@ -3671,14 +3753,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:IW41"/>
+  <dimension ref="A2:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3719,7 +3801,7 @@
     </row>
     <row r="8" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -3748,7 +3830,7 @@
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="12" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="90" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C12" s="90"/>
       <c r="D12" s="90"/>
@@ -3757,17 +3839,17 @@
     </row>
     <row r="14" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="91" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C14" s="91"/>
       <c r="D14" s="91"/>
       <c r="E14" s="91"/>
       <c r="F14" s="91"/>
     </row>
-    <row r="15" s="1" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="15" s="1" customFormat="true" ht="31.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="12"/>
       <c r="B15" s="92" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C15" s="92"/>
       <c r="D15" s="92"/>
@@ -3778,9 +3860,11 @@
       <c r="L15" s="25"/>
       <c r="IW15" s="2"/>
     </row>
-    <row r="16" s="1" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" s="1" customFormat="true" ht="27.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="12"/>
-      <c r="B16" s="92"/>
+      <c r="B16" s="92" t="s">
+        <v>82</v>
+      </c>
       <c r="C16" s="92"/>
       <c r="D16" s="92"/>
       <c r="E16" s="92"/>
@@ -3790,9 +3874,11 @@
       <c r="L16" s="25"/>
       <c r="IW16" s="2"/>
     </row>
-    <row r="17" s="1" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="17" s="1" customFormat="true" ht="25.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="12"/>
-      <c r="B17" s="92"/>
+      <c r="B17" s="92" t="s">
+        <v>83</v>
+      </c>
       <c r="C17" s="92"/>
       <c r="D17" s="92"/>
       <c r="E17" s="92"/>
@@ -3802,9 +3888,11 @@
       <c r="L17" s="25"/>
       <c r="IW17" s="2"/>
     </row>
-    <row r="18" s="1" customFormat="true" ht="58.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="18" s="1" customFormat="true" ht="31.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="12"/>
-      <c r="B18" s="92"/>
+      <c r="B18" s="92" t="s">
+        <v>84</v>
+      </c>
       <c r="C18" s="92"/>
       <c r="D18" s="92"/>
       <c r="E18" s="92"/>
@@ -3816,7 +3904,7 @@
     <row r="19" s="1" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="12"/>
       <c r="B19" s="91" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C19" s="91"/>
       <c r="D19" s="91"/>
@@ -3824,10 +3912,10 @@
       <c r="F19" s="91"/>
       <c r="IW19" s="2"/>
     </row>
-    <row r="20" s="1" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="20" s="1" customFormat="true" ht="55.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="12"/>
       <c r="B20" s="93" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C20" s="93"/>
       <c r="D20" s="93"/>
@@ -3835,164 +3923,934 @@
       <c r="F20" s="93"/>
       <c r="IW20" s="2"/>
     </row>
-    <row r="21" s="1" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="21" s="1" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="12"/>
-      <c r="B21" s="93"/>
+      <c r="B21" s="93" t="s">
+        <v>86</v>
+      </c>
       <c r="C21" s="93"/>
       <c r="D21" s="93"/>
       <c r="E21" s="93"/>
       <c r="F21" s="93"/>
       <c r="IW21" s="2"/>
     </row>
-    <row r="22" s="1" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="22" s="1" customFormat="true" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="12"/>
-      <c r="B22" s="93"/>
+      <c r="B22" s="93" t="s">
+        <v>87</v>
+      </c>
       <c r="C22" s="93"/>
       <c r="D22" s="93"/>
       <c r="E22" s="93"/>
       <c r="F22" s="93"/>
       <c r="IW22" s="2"/>
     </row>
-    <row r="23" s="1" customFormat="true" ht="56.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="23" s="1" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="12"/>
-      <c r="B23" s="93"/>
-      <c r="C23" s="93"/>
-      <c r="D23" s="93"/>
-      <c r="E23" s="93"/>
-      <c r="F23" s="93"/>
+      <c r="B23" s="91" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23" s="91"/>
+      <c r="D23" s="91"/>
+      <c r="E23" s="91"/>
+      <c r="F23" s="91"/>
       <c r="IW23" s="2"/>
     </row>
     <row r="24" s="1" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="12"/>
-      <c r="B24" s="91" t="s">
-        <v>70</v>
-      </c>
-      <c r="C24" s="91"/>
-      <c r="D24" s="91"/>
-      <c r="E24" s="91"/>
-      <c r="F24" s="91"/>
+      <c r="B24" s="92" t="s">
+        <v>88</v>
+      </c>
+      <c r="C24" s="92"/>
+      <c r="D24" s="92"/>
+      <c r="E24" s="92"/>
+      <c r="F24" s="92"/>
       <c r="IW24" s="2"/>
     </row>
-    <row r="25" s="1" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="25" s="1" customFormat="true" ht="52.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="12"/>
-      <c r="B25" s="94" t="s">
-        <v>82</v>
-      </c>
-      <c r="C25" s="94"/>
-      <c r="D25" s="94"/>
-      <c r="E25" s="94"/>
-      <c r="F25" s="94"/>
+      <c r="B25" s="92" t="s">
+        <v>89</v>
+      </c>
+      <c r="C25" s="92"/>
+      <c r="D25" s="92"/>
+      <c r="E25" s="92"/>
+      <c r="F25" s="92"/>
       <c r="IW25" s="2"/>
     </row>
-    <row r="26" s="1" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="26" s="1" customFormat="true" ht="41.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="12"/>
-      <c r="B26" s="94"/>
-      <c r="C26" s="94"/>
-      <c r="D26" s="94"/>
-      <c r="E26" s="94"/>
-      <c r="F26" s="94"/>
+      <c r="B26" s="92" t="s">
+        <v>90</v>
+      </c>
+      <c r="C26" s="92"/>
+      <c r="D26" s="92"/>
+      <c r="E26" s="92"/>
+      <c r="F26" s="92"/>
       <c r="IW26" s="2"/>
     </row>
     <row r="27" s="1" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="12"/>
-      <c r="B27" s="94"/>
-      <c r="C27" s="94"/>
-      <c r="D27" s="94"/>
-      <c r="E27" s="94"/>
-      <c r="F27" s="94"/>
+      <c r="B27" s="92"/>
+      <c r="C27" s="92"/>
+      <c r="D27" s="92"/>
+      <c r="E27" s="92"/>
+      <c r="F27" s="92"/>
       <c r="IW27" s="2"/>
     </row>
     <row r="28" s="1" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B28" s="94"/>
-      <c r="C28" s="94"/>
-      <c r="D28" s="94"/>
-      <c r="E28" s="94"/>
-      <c r="F28" s="94"/>
+      <c r="B28" s="92"/>
+      <c r="C28" s="92"/>
+      <c r="D28" s="92"/>
+      <c r="E28" s="92"/>
+      <c r="F28" s="92"/>
       <c r="IW28" s="2"/>
     </row>
     <row r="29" s="1" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B29" s="94"/>
-      <c r="C29" s="94"/>
-      <c r="D29" s="94"/>
-      <c r="E29" s="94"/>
-      <c r="F29" s="94"/>
+      <c r="B29" s="41"/>
+      <c r="C29" s="41"/>
+      <c r="D29" s="41"/>
       <c r="IW29" s="2"/>
     </row>
     <row r="30" s="1" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B30" s="41"/>
+      <c r="B30" s="49"/>
       <c r="C30" s="41"/>
       <c r="D30" s="41"/>
       <c r="IW30" s="2"/>
     </row>
     <row r="31" s="1" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B31" s="49"/>
+      <c r="B31" s="41"/>
       <c r="C31" s="41"/>
       <c r="D31" s="41"/>
+      <c r="J31" s="50"/>
       <c r="IW31" s="2"/>
     </row>
-    <row r="32" s="1" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B32" s="41"/>
+    <row r="32" s="1" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="49"/>
       <c r="C32" s="41"/>
       <c r="D32" s="41"/>
       <c r="J32" s="50"/>
       <c r="IW32" s="2"/>
     </row>
     <row r="33" s="1" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="49"/>
+      <c r="B33" s="41"/>
       <c r="C33" s="41"/>
       <c r="D33" s="41"/>
-      <c r="J33" s="50"/>
       <c r="IW33" s="2"/>
     </row>
     <row r="34" s="1" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="41"/>
+      <c r="B34" s="49"/>
       <c r="C34" s="41"/>
       <c r="D34" s="41"/>
       <c r="IW34" s="2"/>
     </row>
     <row r="35" s="1" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="49"/>
+      <c r="B35" s="41"/>
       <c r="C35" s="41"/>
       <c r="D35" s="41"/>
       <c r="IW35" s="2"/>
     </row>
     <row r="36" s="1" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="41"/>
+      <c r="B36" s="49"/>
       <c r="C36" s="41"/>
       <c r="D36" s="41"/>
       <c r="IW36" s="2"/>
     </row>
     <row r="37" s="1" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="49"/>
+      <c r="B37" s="41"/>
       <c r="C37" s="41"/>
       <c r="D37" s="41"/>
       <c r="IW37" s="2"/>
     </row>
     <row r="38" s="1" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="41"/>
+      <c r="B38" s="49"/>
       <c r="C38" s="41"/>
       <c r="D38" s="41"/>
       <c r="IW38" s="2"/>
     </row>
     <row r="39" s="1" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="49"/>
+      <c r="B39" s="43"/>
       <c r="C39" s="41"/>
       <c r="D39" s="41"/>
       <c r="IW39" s="2"/>
     </row>
     <row r="40" s="1" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="43"/>
-      <c r="C40" s="41"/>
+      <c r="C40" s="43"/>
       <c r="D40" s="41"/>
       <c r="IW40" s="2"/>
     </row>
     <row r="41" s="1" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C41" s="43"/>
-      <c r="D41" s="41"/>
       <c r="IW41" s="2"/>
-    </row>
+      <c r="IX41" s="2"/>
+      <c r="IY41" s="2"/>
+      <c r="IZ41" s="2"/>
+      <c r="JA41" s="2"/>
+      <c r="JB41" s="2"/>
+      <c r="JC41" s="2"/>
+      <c r="JD41" s="2"/>
+      <c r="JE41" s="2"/>
+      <c r="JF41" s="2"/>
+      <c r="JG41" s="2"/>
+      <c r="JH41" s="2"/>
+      <c r="JI41" s="2"/>
+      <c r="JJ41" s="2"/>
+      <c r="JK41" s="2"/>
+      <c r="JL41" s="2"/>
+      <c r="JM41" s="2"/>
+      <c r="JN41" s="2"/>
+      <c r="JO41" s="2"/>
+      <c r="JP41" s="2"/>
+      <c r="JQ41" s="2"/>
+      <c r="JR41" s="2"/>
+      <c r="JS41" s="2"/>
+      <c r="JT41" s="2"/>
+      <c r="JU41" s="2"/>
+      <c r="JV41" s="2"/>
+      <c r="JW41" s="2"/>
+      <c r="JX41" s="2"/>
+      <c r="JY41" s="2"/>
+      <c r="JZ41" s="2"/>
+      <c r="KA41" s="2"/>
+      <c r="KB41" s="2"/>
+      <c r="KC41" s="2"/>
+      <c r="KD41" s="2"/>
+      <c r="KE41" s="2"/>
+      <c r="KF41" s="2"/>
+      <c r="KG41" s="2"/>
+      <c r="KH41" s="2"/>
+      <c r="KI41" s="2"/>
+      <c r="KJ41" s="2"/>
+      <c r="KK41" s="2"/>
+      <c r="KL41" s="2"/>
+      <c r="KM41" s="2"/>
+      <c r="KN41" s="2"/>
+      <c r="KO41" s="2"/>
+      <c r="KP41" s="2"/>
+      <c r="KQ41" s="2"/>
+      <c r="KR41" s="2"/>
+      <c r="KS41" s="2"/>
+      <c r="KT41" s="2"/>
+      <c r="KU41" s="2"/>
+      <c r="KV41" s="2"/>
+      <c r="KW41" s="2"/>
+      <c r="KX41" s="2"/>
+      <c r="KY41" s="2"/>
+      <c r="KZ41" s="2"/>
+      <c r="LA41" s="2"/>
+      <c r="LB41" s="2"/>
+      <c r="LC41" s="2"/>
+      <c r="LD41" s="2"/>
+      <c r="LE41" s="2"/>
+      <c r="LF41" s="2"/>
+      <c r="LG41" s="2"/>
+      <c r="LH41" s="2"/>
+      <c r="LI41" s="2"/>
+      <c r="LJ41" s="2"/>
+      <c r="LK41" s="2"/>
+      <c r="LL41" s="2"/>
+      <c r="LM41" s="2"/>
+      <c r="LN41" s="2"/>
+      <c r="LO41" s="2"/>
+      <c r="LP41" s="2"/>
+      <c r="LQ41" s="2"/>
+      <c r="LR41" s="2"/>
+      <c r="LS41" s="2"/>
+      <c r="LT41" s="2"/>
+      <c r="LU41" s="2"/>
+      <c r="LV41" s="2"/>
+      <c r="LW41" s="2"/>
+      <c r="LX41" s="2"/>
+      <c r="LY41" s="2"/>
+      <c r="LZ41" s="2"/>
+      <c r="MA41" s="2"/>
+      <c r="MB41" s="2"/>
+      <c r="MC41" s="2"/>
+      <c r="MD41" s="2"/>
+      <c r="ME41" s="2"/>
+      <c r="MF41" s="2"/>
+      <c r="MG41" s="2"/>
+      <c r="MH41" s="2"/>
+      <c r="MI41" s="2"/>
+      <c r="MJ41" s="2"/>
+      <c r="MK41" s="2"/>
+      <c r="ML41" s="2"/>
+      <c r="MM41" s="2"/>
+      <c r="MN41" s="2"/>
+      <c r="MO41" s="2"/>
+      <c r="MP41" s="2"/>
+      <c r="MQ41" s="2"/>
+      <c r="MR41" s="2"/>
+      <c r="MS41" s="2"/>
+      <c r="MT41" s="2"/>
+      <c r="MU41" s="2"/>
+      <c r="MV41" s="2"/>
+      <c r="MW41" s="2"/>
+      <c r="MX41" s="2"/>
+      <c r="MY41" s="2"/>
+      <c r="MZ41" s="2"/>
+      <c r="NA41" s="2"/>
+      <c r="NB41" s="2"/>
+      <c r="NC41" s="2"/>
+      <c r="ND41" s="2"/>
+      <c r="NE41" s="2"/>
+      <c r="NF41" s="2"/>
+      <c r="NG41" s="2"/>
+      <c r="NH41" s="2"/>
+      <c r="NI41" s="2"/>
+      <c r="NJ41" s="2"/>
+      <c r="NK41" s="2"/>
+      <c r="NL41" s="2"/>
+      <c r="NM41" s="2"/>
+      <c r="NN41" s="2"/>
+      <c r="NO41" s="2"/>
+      <c r="NP41" s="2"/>
+      <c r="NQ41" s="2"/>
+      <c r="NR41" s="2"/>
+      <c r="NS41" s="2"/>
+      <c r="NT41" s="2"/>
+      <c r="NU41" s="2"/>
+      <c r="NV41" s="2"/>
+      <c r="NW41" s="2"/>
+      <c r="NX41" s="2"/>
+      <c r="NY41" s="2"/>
+      <c r="NZ41" s="2"/>
+      <c r="OA41" s="2"/>
+      <c r="OB41" s="2"/>
+      <c r="OC41" s="2"/>
+      <c r="OD41" s="2"/>
+      <c r="OE41" s="2"/>
+      <c r="OF41" s="2"/>
+      <c r="OG41" s="2"/>
+      <c r="OH41" s="2"/>
+      <c r="OI41" s="2"/>
+      <c r="OJ41" s="2"/>
+      <c r="OK41" s="2"/>
+      <c r="OL41" s="2"/>
+      <c r="OM41" s="2"/>
+      <c r="ON41" s="2"/>
+      <c r="OO41" s="2"/>
+      <c r="OP41" s="2"/>
+      <c r="OQ41" s="2"/>
+      <c r="OR41" s="2"/>
+      <c r="OS41" s="2"/>
+      <c r="OT41" s="2"/>
+      <c r="OU41" s="2"/>
+      <c r="OV41" s="2"/>
+      <c r="OW41" s="2"/>
+      <c r="OX41" s="2"/>
+      <c r="OY41" s="2"/>
+      <c r="OZ41" s="2"/>
+      <c r="PA41" s="2"/>
+      <c r="PB41" s="2"/>
+      <c r="PC41" s="2"/>
+      <c r="PD41" s="2"/>
+      <c r="PE41" s="2"/>
+      <c r="PF41" s="2"/>
+      <c r="PG41" s="2"/>
+      <c r="PH41" s="2"/>
+      <c r="PI41" s="2"/>
+      <c r="PJ41" s="2"/>
+      <c r="PK41" s="2"/>
+      <c r="PL41" s="2"/>
+      <c r="PM41" s="2"/>
+      <c r="PN41" s="2"/>
+      <c r="PO41" s="2"/>
+      <c r="PP41" s="2"/>
+      <c r="PQ41" s="2"/>
+      <c r="PR41" s="2"/>
+      <c r="PS41" s="2"/>
+      <c r="PT41" s="2"/>
+      <c r="PU41" s="2"/>
+      <c r="PV41" s="2"/>
+      <c r="PW41" s="2"/>
+      <c r="PX41" s="2"/>
+      <c r="PY41" s="2"/>
+      <c r="PZ41" s="2"/>
+      <c r="QA41" s="2"/>
+      <c r="QB41" s="2"/>
+      <c r="QC41" s="2"/>
+      <c r="QD41" s="2"/>
+      <c r="QE41" s="2"/>
+      <c r="QF41" s="2"/>
+      <c r="QG41" s="2"/>
+      <c r="QH41" s="2"/>
+      <c r="QI41" s="2"/>
+      <c r="QJ41" s="2"/>
+      <c r="QK41" s="2"/>
+      <c r="QL41" s="2"/>
+      <c r="QM41" s="2"/>
+      <c r="QN41" s="2"/>
+      <c r="QO41" s="2"/>
+      <c r="QP41" s="2"/>
+      <c r="QQ41" s="2"/>
+      <c r="QR41" s="2"/>
+      <c r="QS41" s="2"/>
+      <c r="QT41" s="2"/>
+      <c r="QU41" s="2"/>
+      <c r="QV41" s="2"/>
+      <c r="QW41" s="2"/>
+      <c r="QX41" s="2"/>
+      <c r="QY41" s="2"/>
+      <c r="QZ41" s="2"/>
+      <c r="RA41" s="2"/>
+      <c r="RB41" s="2"/>
+      <c r="RC41" s="2"/>
+      <c r="RD41" s="2"/>
+      <c r="RE41" s="2"/>
+      <c r="RF41" s="2"/>
+      <c r="RG41" s="2"/>
+      <c r="RH41" s="2"/>
+      <c r="RI41" s="2"/>
+      <c r="RJ41" s="2"/>
+      <c r="RK41" s="2"/>
+      <c r="RL41" s="2"/>
+      <c r="RM41" s="2"/>
+      <c r="RN41" s="2"/>
+      <c r="RO41" s="2"/>
+      <c r="RP41" s="2"/>
+      <c r="RQ41" s="2"/>
+      <c r="RR41" s="2"/>
+      <c r="RS41" s="2"/>
+      <c r="RT41" s="2"/>
+      <c r="RU41" s="2"/>
+      <c r="RV41" s="2"/>
+      <c r="RW41" s="2"/>
+      <c r="RX41" s="2"/>
+      <c r="RY41" s="2"/>
+      <c r="RZ41" s="2"/>
+      <c r="SA41" s="2"/>
+      <c r="SB41" s="2"/>
+      <c r="SC41" s="2"/>
+      <c r="SD41" s="2"/>
+      <c r="SE41" s="2"/>
+      <c r="SF41" s="2"/>
+      <c r="SG41" s="2"/>
+      <c r="SH41" s="2"/>
+      <c r="SI41" s="2"/>
+      <c r="SJ41" s="2"/>
+      <c r="SK41" s="2"/>
+      <c r="SL41" s="2"/>
+      <c r="SM41" s="2"/>
+      <c r="SN41" s="2"/>
+      <c r="SO41" s="2"/>
+      <c r="SP41" s="2"/>
+      <c r="SQ41" s="2"/>
+      <c r="SR41" s="2"/>
+      <c r="SS41" s="2"/>
+      <c r="ST41" s="2"/>
+      <c r="SU41" s="2"/>
+      <c r="SV41" s="2"/>
+      <c r="SW41" s="2"/>
+      <c r="SX41" s="2"/>
+      <c r="SY41" s="2"/>
+      <c r="SZ41" s="2"/>
+      <c r="TA41" s="2"/>
+      <c r="TB41" s="2"/>
+      <c r="TC41" s="2"/>
+      <c r="TD41" s="2"/>
+      <c r="TE41" s="2"/>
+      <c r="TF41" s="2"/>
+      <c r="TG41" s="2"/>
+      <c r="TH41" s="2"/>
+      <c r="TI41" s="2"/>
+      <c r="TJ41" s="2"/>
+      <c r="TK41" s="2"/>
+      <c r="TL41" s="2"/>
+      <c r="TM41" s="2"/>
+      <c r="TN41" s="2"/>
+      <c r="TO41" s="2"/>
+      <c r="TP41" s="2"/>
+      <c r="TQ41" s="2"/>
+      <c r="TR41" s="2"/>
+      <c r="TS41" s="2"/>
+      <c r="TT41" s="2"/>
+      <c r="TU41" s="2"/>
+      <c r="TV41" s="2"/>
+      <c r="TW41" s="2"/>
+      <c r="TX41" s="2"/>
+      <c r="TY41" s="2"/>
+      <c r="TZ41" s="2"/>
+      <c r="UA41" s="2"/>
+      <c r="UB41" s="2"/>
+      <c r="UC41" s="2"/>
+      <c r="UD41" s="2"/>
+      <c r="UE41" s="2"/>
+      <c r="UF41" s="2"/>
+      <c r="UG41" s="2"/>
+      <c r="UH41" s="2"/>
+      <c r="UI41" s="2"/>
+      <c r="UJ41" s="2"/>
+      <c r="UK41" s="2"/>
+      <c r="UL41" s="2"/>
+      <c r="UM41" s="2"/>
+      <c r="UN41" s="2"/>
+      <c r="UO41" s="2"/>
+      <c r="UP41" s="2"/>
+      <c r="UQ41" s="2"/>
+      <c r="UR41" s="2"/>
+      <c r="US41" s="2"/>
+      <c r="UT41" s="2"/>
+      <c r="UU41" s="2"/>
+      <c r="UV41" s="2"/>
+      <c r="UW41" s="2"/>
+      <c r="UX41" s="2"/>
+      <c r="UY41" s="2"/>
+      <c r="UZ41" s="2"/>
+      <c r="VA41" s="2"/>
+      <c r="VB41" s="2"/>
+      <c r="VC41" s="2"/>
+      <c r="VD41" s="2"/>
+      <c r="VE41" s="2"/>
+      <c r="VF41" s="2"/>
+      <c r="VG41" s="2"/>
+      <c r="VH41" s="2"/>
+      <c r="VI41" s="2"/>
+      <c r="VJ41" s="2"/>
+      <c r="VK41" s="2"/>
+      <c r="VL41" s="2"/>
+      <c r="VM41" s="2"/>
+      <c r="VN41" s="2"/>
+      <c r="VO41" s="2"/>
+      <c r="VP41" s="2"/>
+      <c r="VQ41" s="2"/>
+      <c r="VR41" s="2"/>
+      <c r="VS41" s="2"/>
+      <c r="VT41" s="2"/>
+      <c r="VU41" s="2"/>
+      <c r="VV41" s="2"/>
+      <c r="VW41" s="2"/>
+      <c r="VX41" s="2"/>
+      <c r="VY41" s="2"/>
+      <c r="VZ41" s="2"/>
+      <c r="WA41" s="2"/>
+      <c r="WB41" s="2"/>
+      <c r="WC41" s="2"/>
+      <c r="WD41" s="2"/>
+      <c r="WE41" s="2"/>
+      <c r="WF41" s="2"/>
+      <c r="WG41" s="2"/>
+      <c r="WH41" s="2"/>
+      <c r="WI41" s="2"/>
+      <c r="WJ41" s="2"/>
+      <c r="WK41" s="2"/>
+      <c r="WL41" s="2"/>
+      <c r="WM41" s="2"/>
+      <c r="WN41" s="2"/>
+      <c r="WO41" s="2"/>
+      <c r="WP41" s="2"/>
+      <c r="WQ41" s="2"/>
+      <c r="WR41" s="2"/>
+      <c r="WS41" s="2"/>
+      <c r="WT41" s="2"/>
+      <c r="WU41" s="2"/>
+      <c r="WV41" s="2"/>
+      <c r="WW41" s="2"/>
+      <c r="WX41" s="2"/>
+      <c r="WY41" s="2"/>
+      <c r="WZ41" s="2"/>
+      <c r="XA41" s="2"/>
+      <c r="XB41" s="2"/>
+      <c r="XC41" s="2"/>
+      <c r="XD41" s="2"/>
+      <c r="XE41" s="2"/>
+      <c r="XF41" s="2"/>
+      <c r="XG41" s="2"/>
+      <c r="XH41" s="2"/>
+      <c r="XI41" s="2"/>
+      <c r="XJ41" s="2"/>
+      <c r="XK41" s="2"/>
+      <c r="XL41" s="2"/>
+      <c r="XM41" s="2"/>
+      <c r="XN41" s="2"/>
+      <c r="XO41" s="2"/>
+      <c r="XP41" s="2"/>
+      <c r="XQ41" s="2"/>
+      <c r="XR41" s="2"/>
+      <c r="XS41" s="2"/>
+      <c r="XT41" s="2"/>
+      <c r="XU41" s="2"/>
+      <c r="XV41" s="2"/>
+      <c r="XW41" s="2"/>
+      <c r="XX41" s="2"/>
+      <c r="XY41" s="2"/>
+      <c r="XZ41" s="2"/>
+      <c r="YA41" s="2"/>
+      <c r="YB41" s="2"/>
+      <c r="YC41" s="2"/>
+      <c r="YD41" s="2"/>
+      <c r="YE41" s="2"/>
+      <c r="YF41" s="2"/>
+      <c r="YG41" s="2"/>
+      <c r="YH41" s="2"/>
+      <c r="YI41" s="2"/>
+      <c r="YJ41" s="2"/>
+      <c r="YK41" s="2"/>
+      <c r="YL41" s="2"/>
+      <c r="YM41" s="2"/>
+      <c r="YN41" s="2"/>
+      <c r="YO41" s="2"/>
+      <c r="YP41" s="2"/>
+      <c r="YQ41" s="2"/>
+      <c r="YR41" s="2"/>
+      <c r="YS41" s="2"/>
+      <c r="YT41" s="2"/>
+      <c r="YU41" s="2"/>
+      <c r="YV41" s="2"/>
+      <c r="YW41" s="2"/>
+      <c r="YX41" s="2"/>
+      <c r="YY41" s="2"/>
+      <c r="YZ41" s="2"/>
+      <c r="ZA41" s="2"/>
+      <c r="ZB41" s="2"/>
+      <c r="ZC41" s="2"/>
+      <c r="ZD41" s="2"/>
+      <c r="ZE41" s="2"/>
+      <c r="ZF41" s="2"/>
+      <c r="ZG41" s="2"/>
+      <c r="ZH41" s="2"/>
+      <c r="ZI41" s="2"/>
+      <c r="ZJ41" s="2"/>
+      <c r="ZK41" s="2"/>
+      <c r="ZL41" s="2"/>
+      <c r="ZM41" s="2"/>
+      <c r="ZN41" s="2"/>
+      <c r="ZO41" s="2"/>
+      <c r="ZP41" s="2"/>
+      <c r="ZQ41" s="2"/>
+      <c r="ZR41" s="2"/>
+      <c r="ZS41" s="2"/>
+      <c r="ZT41" s="2"/>
+      <c r="ZU41" s="2"/>
+      <c r="ZV41" s="2"/>
+      <c r="ZW41" s="2"/>
+      <c r="ZX41" s="2"/>
+      <c r="ZY41" s="2"/>
+      <c r="ZZ41" s="2"/>
+      <c r="AAA41" s="2"/>
+      <c r="AAB41" s="2"/>
+      <c r="AAC41" s="2"/>
+      <c r="AAD41" s="2"/>
+      <c r="AAE41" s="2"/>
+      <c r="AAF41" s="2"/>
+      <c r="AAG41" s="2"/>
+      <c r="AAH41" s="2"/>
+      <c r="AAI41" s="2"/>
+      <c r="AAJ41" s="2"/>
+      <c r="AAK41" s="2"/>
+      <c r="AAL41" s="2"/>
+      <c r="AAM41" s="2"/>
+      <c r="AAN41" s="2"/>
+      <c r="AAO41" s="2"/>
+      <c r="AAP41" s="2"/>
+      <c r="AAQ41" s="2"/>
+      <c r="AAR41" s="2"/>
+      <c r="AAS41" s="2"/>
+      <c r="AAT41" s="2"/>
+      <c r="AAU41" s="2"/>
+      <c r="AAV41" s="2"/>
+      <c r="AAW41" s="2"/>
+      <c r="AAX41" s="2"/>
+      <c r="AAY41" s="2"/>
+      <c r="AAZ41" s="2"/>
+      <c r="ABA41" s="2"/>
+      <c r="ABB41" s="2"/>
+      <c r="ABC41" s="2"/>
+      <c r="ABD41" s="2"/>
+      <c r="ABE41" s="2"/>
+      <c r="ABF41" s="2"/>
+      <c r="ABG41" s="2"/>
+      <c r="ABH41" s="2"/>
+      <c r="ABI41" s="2"/>
+      <c r="ABJ41" s="2"/>
+      <c r="ABK41" s="2"/>
+      <c r="ABL41" s="2"/>
+      <c r="ABM41" s="2"/>
+      <c r="ABN41" s="2"/>
+      <c r="ABO41" s="2"/>
+      <c r="ABP41" s="2"/>
+      <c r="ABQ41" s="2"/>
+      <c r="ABR41" s="2"/>
+      <c r="ABS41" s="2"/>
+      <c r="ABT41" s="2"/>
+      <c r="ABU41" s="2"/>
+      <c r="ABV41" s="2"/>
+      <c r="ABW41" s="2"/>
+      <c r="ABX41" s="2"/>
+      <c r="ABY41" s="2"/>
+      <c r="ABZ41" s="2"/>
+      <c r="ACA41" s="2"/>
+      <c r="ACB41" s="2"/>
+      <c r="ACC41" s="2"/>
+      <c r="ACD41" s="2"/>
+      <c r="ACE41" s="2"/>
+      <c r="ACF41" s="2"/>
+      <c r="ACG41" s="2"/>
+      <c r="ACH41" s="2"/>
+      <c r="ACI41" s="2"/>
+      <c r="ACJ41" s="2"/>
+      <c r="ACK41" s="2"/>
+      <c r="ACL41" s="2"/>
+      <c r="ACM41" s="2"/>
+      <c r="ACN41" s="2"/>
+      <c r="ACO41" s="2"/>
+      <c r="ACP41" s="2"/>
+      <c r="ACQ41" s="2"/>
+      <c r="ACR41" s="2"/>
+      <c r="ACS41" s="2"/>
+      <c r="ACT41" s="2"/>
+      <c r="ACU41" s="2"/>
+      <c r="ACV41" s="2"/>
+      <c r="ACW41" s="2"/>
+      <c r="ACX41" s="2"/>
+      <c r="ACY41" s="2"/>
+      <c r="ACZ41" s="2"/>
+      <c r="ADA41" s="2"/>
+      <c r="ADB41" s="2"/>
+      <c r="ADC41" s="2"/>
+      <c r="ADD41" s="2"/>
+      <c r="ADE41" s="2"/>
+      <c r="ADF41" s="2"/>
+      <c r="ADG41" s="2"/>
+      <c r="ADH41" s="2"/>
+      <c r="ADI41" s="2"/>
+      <c r="ADJ41" s="2"/>
+      <c r="ADK41" s="2"/>
+      <c r="ADL41" s="2"/>
+      <c r="ADM41" s="2"/>
+      <c r="ADN41" s="2"/>
+      <c r="ADO41" s="2"/>
+      <c r="ADP41" s="2"/>
+      <c r="ADQ41" s="2"/>
+      <c r="ADR41" s="2"/>
+      <c r="ADS41" s="2"/>
+      <c r="ADT41" s="2"/>
+      <c r="ADU41" s="2"/>
+      <c r="ADV41" s="2"/>
+      <c r="ADW41" s="2"/>
+      <c r="ADX41" s="2"/>
+      <c r="ADY41" s="2"/>
+      <c r="ADZ41" s="2"/>
+      <c r="AEA41" s="2"/>
+      <c r="AEB41" s="2"/>
+      <c r="AEC41" s="2"/>
+      <c r="AED41" s="2"/>
+      <c r="AEE41" s="2"/>
+      <c r="AEF41" s="2"/>
+      <c r="AEG41" s="2"/>
+      <c r="AEH41" s="2"/>
+      <c r="AEI41" s="2"/>
+      <c r="AEJ41" s="2"/>
+      <c r="AEK41" s="2"/>
+      <c r="AEL41" s="2"/>
+      <c r="AEM41" s="2"/>
+      <c r="AEN41" s="2"/>
+      <c r="AEO41" s="2"/>
+      <c r="AEP41" s="2"/>
+      <c r="AEQ41" s="2"/>
+      <c r="AER41" s="2"/>
+      <c r="AES41" s="2"/>
+      <c r="AET41" s="2"/>
+      <c r="AEU41" s="2"/>
+      <c r="AEV41" s="2"/>
+      <c r="AEW41" s="2"/>
+      <c r="AEX41" s="2"/>
+      <c r="AEY41" s="2"/>
+      <c r="AEZ41" s="2"/>
+      <c r="AFA41" s="2"/>
+      <c r="AFB41" s="2"/>
+      <c r="AFC41" s="2"/>
+      <c r="AFD41" s="2"/>
+      <c r="AFE41" s="2"/>
+      <c r="AFF41" s="2"/>
+      <c r="AFG41" s="2"/>
+      <c r="AFH41" s="2"/>
+      <c r="AFI41" s="2"/>
+      <c r="AFJ41" s="2"/>
+      <c r="AFK41" s="2"/>
+      <c r="AFL41" s="2"/>
+      <c r="AFM41" s="2"/>
+      <c r="AFN41" s="2"/>
+      <c r="AFO41" s="2"/>
+      <c r="AFP41" s="2"/>
+      <c r="AFQ41" s="2"/>
+      <c r="AFR41" s="2"/>
+      <c r="AFS41" s="2"/>
+      <c r="AFT41" s="2"/>
+      <c r="AFU41" s="2"/>
+      <c r="AFV41" s="2"/>
+      <c r="AFW41" s="2"/>
+      <c r="AFX41" s="2"/>
+      <c r="AFY41" s="2"/>
+      <c r="AFZ41" s="2"/>
+      <c r="AGA41" s="2"/>
+      <c r="AGB41" s="2"/>
+      <c r="AGC41" s="2"/>
+      <c r="AGD41" s="2"/>
+      <c r="AGE41" s="2"/>
+      <c r="AGF41" s="2"/>
+      <c r="AGG41" s="2"/>
+      <c r="AGH41" s="2"/>
+      <c r="AGI41" s="2"/>
+      <c r="AGJ41" s="2"/>
+      <c r="AGK41" s="2"/>
+      <c r="AGL41" s="2"/>
+      <c r="AGM41" s="2"/>
+      <c r="AGN41" s="2"/>
+      <c r="AGO41" s="2"/>
+      <c r="AGP41" s="2"/>
+      <c r="AGQ41" s="2"/>
+      <c r="AGR41" s="2"/>
+      <c r="AGS41" s="2"/>
+      <c r="AGT41" s="2"/>
+      <c r="AGU41" s="2"/>
+      <c r="AGV41" s="2"/>
+      <c r="AGW41" s="2"/>
+      <c r="AGX41" s="2"/>
+      <c r="AGY41" s="2"/>
+      <c r="AGZ41" s="2"/>
+      <c r="AHA41" s="2"/>
+      <c r="AHB41" s="2"/>
+      <c r="AHC41" s="2"/>
+      <c r="AHD41" s="2"/>
+      <c r="AHE41" s="2"/>
+      <c r="AHF41" s="2"/>
+      <c r="AHG41" s="2"/>
+      <c r="AHH41" s="2"/>
+      <c r="AHI41" s="2"/>
+      <c r="AHJ41" s="2"/>
+      <c r="AHK41" s="2"/>
+      <c r="AHL41" s="2"/>
+      <c r="AHM41" s="2"/>
+      <c r="AHN41" s="2"/>
+      <c r="AHO41" s="2"/>
+      <c r="AHP41" s="2"/>
+      <c r="AHQ41" s="2"/>
+      <c r="AHR41" s="2"/>
+      <c r="AHS41" s="2"/>
+      <c r="AHT41" s="2"/>
+      <c r="AHU41" s="2"/>
+      <c r="AHV41" s="2"/>
+      <c r="AHW41" s="2"/>
+      <c r="AHX41" s="2"/>
+      <c r="AHY41" s="2"/>
+      <c r="AHZ41" s="2"/>
+      <c r="AIA41" s="2"/>
+      <c r="AIB41" s="2"/>
+      <c r="AIC41" s="2"/>
+      <c r="AID41" s="2"/>
+      <c r="AIE41" s="2"/>
+      <c r="AIF41" s="2"/>
+      <c r="AIG41" s="2"/>
+      <c r="AIH41" s="2"/>
+      <c r="AII41" s="2"/>
+      <c r="AIJ41" s="2"/>
+      <c r="AIK41" s="2"/>
+      <c r="AIL41" s="2"/>
+      <c r="AIM41" s="2"/>
+      <c r="AIN41" s="2"/>
+      <c r="AIO41" s="2"/>
+      <c r="AIP41" s="2"/>
+      <c r="AIQ41" s="2"/>
+      <c r="AIR41" s="2"/>
+      <c r="AIS41" s="2"/>
+      <c r="AIT41" s="2"/>
+      <c r="AIU41" s="2"/>
+      <c r="AIV41" s="2"/>
+      <c r="AIW41" s="2"/>
+      <c r="AIX41" s="2"/>
+      <c r="AIY41" s="2"/>
+      <c r="AIZ41" s="2"/>
+      <c r="AJA41" s="2"/>
+      <c r="AJB41" s="2"/>
+      <c r="AJC41" s="2"/>
+      <c r="AJD41" s="2"/>
+      <c r="AJE41" s="2"/>
+      <c r="AJF41" s="2"/>
+      <c r="AJG41" s="2"/>
+      <c r="AJH41" s="2"/>
+      <c r="AJI41" s="2"/>
+      <c r="AJJ41" s="2"/>
+      <c r="AJK41" s="2"/>
+      <c r="AJL41" s="2"/>
+      <c r="AJM41" s="2"/>
+      <c r="AJN41" s="2"/>
+      <c r="AJO41" s="2"/>
+      <c r="AJP41" s="2"/>
+      <c r="AJQ41" s="2"/>
+      <c r="AJR41" s="2"/>
+      <c r="AJS41" s="2"/>
+      <c r="AJT41" s="2"/>
+      <c r="AJU41" s="2"/>
+      <c r="AJV41" s="2"/>
+      <c r="AJW41" s="2"/>
+      <c r="AJX41" s="2"/>
+      <c r="AJY41" s="2"/>
+      <c r="AJZ41" s="2"/>
+      <c r="AKA41" s="2"/>
+      <c r="AKB41" s="2"/>
+      <c r="AKC41" s="2"/>
+      <c r="AKD41" s="2"/>
+      <c r="AKE41" s="2"/>
+      <c r="AKF41" s="2"/>
+      <c r="AKG41" s="2"/>
+      <c r="AKH41" s="2"/>
+      <c r="AKI41" s="2"/>
+      <c r="AKJ41" s="2"/>
+      <c r="AKK41" s="2"/>
+      <c r="AKL41" s="2"/>
+      <c r="AKM41" s="2"/>
+      <c r="AKN41" s="2"/>
+      <c r="AKO41" s="2"/>
+      <c r="AKP41" s="2"/>
+      <c r="AKQ41" s="2"/>
+      <c r="AKR41" s="2"/>
+      <c r="AKS41" s="2"/>
+      <c r="AKT41" s="2"/>
+      <c r="AKU41" s="2"/>
+      <c r="AKV41" s="2"/>
+      <c r="AKW41" s="2"/>
+      <c r="AKX41" s="2"/>
+      <c r="AKY41" s="2"/>
+      <c r="AKZ41" s="2"/>
+      <c r="ALA41" s="2"/>
+      <c r="ALB41" s="2"/>
+      <c r="ALC41" s="2"/>
+      <c r="ALD41" s="2"/>
+      <c r="ALE41" s="2"/>
+      <c r="ALF41" s="2"/>
+      <c r="ALG41" s="2"/>
+      <c r="ALH41" s="2"/>
+      <c r="ALI41" s="2"/>
+      <c r="ALJ41" s="2"/>
+      <c r="ALK41" s="2"/>
+      <c r="ALL41" s="2"/>
+      <c r="ALM41" s="2"/>
+      <c r="ALN41" s="2"/>
+      <c r="ALO41" s="2"/>
+      <c r="ALP41" s="2"/>
+      <c r="ALQ41" s="2"/>
+      <c r="ALR41" s="2"/>
+      <c r="ALS41" s="2"/>
+      <c r="ALT41" s="2"/>
+      <c r="ALU41" s="2"/>
+      <c r="ALV41" s="2"/>
+      <c r="ALW41" s="2"/>
+      <c r="ALX41" s="2"/>
+      <c r="ALY41" s="2"/>
+      <c r="ALZ41" s="2"/>
+      <c r="AMA41" s="2"/>
+      <c r="AMB41" s="2"/>
+      <c r="AMC41" s="2"/>
+      <c r="AMD41" s="2"/>
+      <c r="AME41" s="2"/>
+      <c r="AMF41" s="2"/>
+      <c r="AMG41" s="2"/>
+      <c r="AMH41" s="2"/>
+      <c r="AMI41" s="2"/>
+      <c r="AMJ41" s="2"/>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="20">
     <mergeCell ref="C5:E5"/>
     <mergeCell ref="F5:H5"/>
     <mergeCell ref="C6:E6"/>
@@ -4001,11 +4859,18 @@
     <mergeCell ref="A10:K10"/>
     <mergeCell ref="B12:F12"/>
     <mergeCell ref="B14:F14"/>
-    <mergeCell ref="B15:F18"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B18:F18"/>
     <mergeCell ref="B19:F19"/>
-    <mergeCell ref="B20:F23"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B23:F23"/>
     <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B25:F29"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="B26:F26"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
   <pageMargins left="0" right="0" top="0.0395833333333333" bottom="0.0395833333333333" header="0.511811023622047" footer="0.511811023622047"/>
@@ -4019,14 +4884,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:IV41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D34" activeCellId="0" sqref="D34"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G30" activeCellId="0" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4097,7 +4962,7 @@
     </row>
     <row r="8" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -4137,77 +5002,91 @@
       <c r="IV11" s="1"/>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F12" s="95"/>
+      <c r="F12" s="94"/>
+    </row>
+    <row r="13" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="91" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" s="91"/>
+      <c r="D13" s="91"/>
+      <c r="E13" s="91"/>
+      <c r="F13" s="91"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B14" s="95" t="s">
+        <v>92</v>
+      </c>
+      <c r="C14" s="95"/>
+      <c r="D14" s="95"/>
+      <c r="E14" s="95"/>
+      <c r="F14" s="95"/>
     </row>
     <row r="15" s="1" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="12"/>
-      <c r="B15" s="49"/>
-      <c r="C15" s="41"/>
-      <c r="D15" s="41"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="42"/>
+      <c r="B15" s="95"/>
+      <c r="C15" s="95"/>
+      <c r="D15" s="95"/>
+      <c r="E15" s="95"/>
+      <c r="F15" s="95"/>
       <c r="G15" s="41"/>
       <c r="K15" s="25"/>
       <c r="IT15" s="2"/>
     </row>
-    <row r="16" s="1" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" s="1" customFormat="true" ht="45.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="12"/>
-      <c r="B16" s="91" t="s">
-        <v>60</v>
-      </c>
-      <c r="C16" s="91"/>
-      <c r="D16" s="91"/>
-      <c r="E16" s="91"/>
-      <c r="F16" s="91"/>
+      <c r="B16" s="95"/>
+      <c r="C16" s="95"/>
+      <c r="D16" s="95"/>
+      <c r="E16" s="95"/>
+      <c r="F16" s="95"/>
       <c r="G16" s="41"/>
       <c r="K16" s="25"/>
       <c r="IT16" s="2"/>
     </row>
-    <row r="17" s="1" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="17" s="1" customFormat="true" ht="43.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="12"/>
-      <c r="B17" s="96" t="s">
-        <v>84</v>
-      </c>
-      <c r="C17" s="96"/>
-      <c r="D17" s="96"/>
-      <c r="E17" s="96"/>
-      <c r="F17" s="96"/>
+      <c r="B17" s="95"/>
+      <c r="C17" s="95"/>
+      <c r="D17" s="95"/>
+      <c r="E17" s="95"/>
+      <c r="F17" s="95"/>
       <c r="G17" s="41"/>
       <c r="K17" s="25"/>
       <c r="IT17" s="2"/>
     </row>
     <row r="18" s="1" customFormat="true" ht="45.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="12"/>
-      <c r="B18" s="96"/>
-      <c r="C18" s="96"/>
-      <c r="D18" s="96"/>
-      <c r="E18" s="96"/>
-      <c r="F18" s="96"/>
+      <c r="B18" s="95"/>
+      <c r="C18" s="95"/>
+      <c r="D18" s="95"/>
+      <c r="E18" s="95"/>
+      <c r="F18" s="95"/>
       <c r="K18" s="25"/>
       <c r="IT18" s="2"/>
     </row>
-    <row r="19" s="1" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="19" s="1" customFormat="true" ht="51.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="12"/>
-      <c r="B19" s="96"/>
-      <c r="C19" s="96"/>
-      <c r="D19" s="96"/>
-      <c r="E19" s="96"/>
-      <c r="F19" s="96"/>
+      <c r="B19" s="95"/>
+      <c r="C19" s="95"/>
+      <c r="D19" s="95"/>
+      <c r="E19" s="95"/>
+      <c r="F19" s="95"/>
       <c r="IT19" s="2"/>
     </row>
-    <row r="20" s="1" customFormat="true" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="20" s="1" customFormat="true" ht="77.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="12"/>
-      <c r="B20" s="96"/>
-      <c r="C20" s="96"/>
-      <c r="D20" s="96"/>
-      <c r="E20" s="96"/>
-      <c r="F20" s="96"/>
+      <c r="B20" s="95"/>
+      <c r="C20" s="95"/>
+      <c r="D20" s="95"/>
+      <c r="E20" s="95"/>
+      <c r="F20" s="95"/>
       <c r="IT20" s="2"/>
     </row>
     <row r="21" s="1" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="12"/>
       <c r="B21" s="91" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C21" s="91"/>
       <c r="D21" s="91"/>
@@ -4215,50 +5094,50 @@
       <c r="F21" s="91"/>
       <c r="IT21" s="2"/>
     </row>
-    <row r="22" s="1" customFormat="true" ht="47.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="22" s="1" customFormat="true" ht="89.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="12"/>
-      <c r="B22" s="97" t="s">
-        <v>85</v>
-      </c>
-      <c r="C22" s="97"/>
-      <c r="D22" s="97"/>
-      <c r="E22" s="97"/>
-      <c r="F22" s="97"/>
+      <c r="B22" s="96" t="s">
+        <v>93</v>
+      </c>
+      <c r="C22" s="96"/>
+      <c r="D22" s="96"/>
+      <c r="E22" s="96"/>
+      <c r="F22" s="96"/>
       <c r="IT22" s="2"/>
     </row>
-    <row r="23" s="1" customFormat="true" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="23" s="1" customFormat="true" ht="91.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="12"/>
-      <c r="B23" s="97"/>
-      <c r="C23" s="97"/>
-      <c r="D23" s="97"/>
-      <c r="E23" s="97"/>
-      <c r="F23" s="97"/>
+      <c r="B23" s="96"/>
+      <c r="C23" s="96"/>
+      <c r="D23" s="96"/>
+      <c r="E23" s="96"/>
+      <c r="F23" s="96"/>
       <c r="IT23" s="2"/>
     </row>
-    <row r="24" s="1" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="24" s="1" customFormat="true" ht="110.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="12"/>
-      <c r="B24" s="97" t="s">
-        <v>86</v>
-      </c>
-      <c r="C24" s="97"/>
-      <c r="D24" s="97"/>
-      <c r="E24" s="97"/>
-      <c r="F24" s="97"/>
+      <c r="B24" s="96" t="s">
+        <v>94</v>
+      </c>
+      <c r="C24" s="96"/>
+      <c r="D24" s="96"/>
+      <c r="E24" s="96"/>
+      <c r="F24" s="96"/>
       <c r="IT24" s="2"/>
     </row>
-    <row r="25" s="1" customFormat="true" ht="42.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="25" s="1" customFormat="true" ht="65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="12"/>
-      <c r="B25" s="97"/>
-      <c r="C25" s="97"/>
-      <c r="D25" s="97"/>
-      <c r="E25" s="97"/>
-      <c r="F25" s="97"/>
+      <c r="B25" s="96"/>
+      <c r="C25" s="96"/>
+      <c r="D25" s="96"/>
+      <c r="E25" s="96"/>
+      <c r="F25" s="96"/>
       <c r="IT25" s="2"/>
     </row>
     <row r="26" s="1" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="12"/>
       <c r="B26" s="91" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C26" s="91"/>
       <c r="D26" s="91"/>
@@ -4266,47 +5145,47 @@
       <c r="F26" s="91"/>
       <c r="IT26" s="2"/>
     </row>
-    <row r="27" s="1" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="27" s="1" customFormat="true" ht="91.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="12"/>
-      <c r="B27" s="94" t="s">
-        <v>87</v>
-      </c>
-      <c r="C27" s="94"/>
-      <c r="D27" s="94"/>
-      <c r="E27" s="94"/>
-      <c r="F27" s="94"/>
+      <c r="B27" s="97" t="s">
+        <v>95</v>
+      </c>
+      <c r="C27" s="97"/>
+      <c r="D27" s="97"/>
+      <c r="E27" s="97"/>
+      <c r="F27" s="97"/>
       <c r="IT27" s="2"/>
     </row>
-    <row r="28" s="1" customFormat="true" ht="46.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B28" s="94"/>
-      <c r="C28" s="94"/>
-      <c r="D28" s="94"/>
-      <c r="E28" s="94"/>
-      <c r="F28" s="94"/>
+    <row r="28" s="1" customFormat="true" ht="75.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B28" s="97"/>
+      <c r="C28" s="97"/>
+      <c r="D28" s="97"/>
+      <c r="E28" s="97"/>
+      <c r="F28" s="97"/>
       <c r="IT28" s="2"/>
     </row>
-    <row r="29" s="1" customFormat="true" ht="44.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B29" s="94"/>
-      <c r="C29" s="94"/>
-      <c r="D29" s="94"/>
-      <c r="E29" s="94"/>
-      <c r="F29" s="94"/>
+    <row r="29" s="1" customFormat="true" ht="76.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B29" s="97"/>
+      <c r="C29" s="97"/>
+      <c r="D29" s="97"/>
+      <c r="E29" s="97"/>
+      <c r="F29" s="97"/>
       <c r="IT29" s="2"/>
     </row>
-    <row r="30" s="1" customFormat="true" ht="51.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B30" s="94"/>
-      <c r="C30" s="94"/>
-      <c r="D30" s="94"/>
-      <c r="E30" s="94"/>
-      <c r="F30" s="94"/>
+    <row r="30" s="1" customFormat="true" ht="94.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B30" s="97"/>
+      <c r="C30" s="97"/>
+      <c r="D30" s="97"/>
+      <c r="E30" s="97"/>
+      <c r="F30" s="97"/>
       <c r="IT30" s="2"/>
     </row>
-    <row r="31" s="1" customFormat="true" ht="39.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B31" s="94"/>
-      <c r="C31" s="94"/>
-      <c r="D31" s="94"/>
-      <c r="E31" s="94"/>
-      <c r="F31" s="94"/>
+    <row r="31" s="1" customFormat="true" ht="74.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B31" s="97"/>
+      <c r="C31" s="97"/>
+      <c r="D31" s="97"/>
+      <c r="E31" s="97"/>
+      <c r="F31" s="97"/>
       <c r="IT31" s="2"/>
     </row>
     <row r="32" s="1" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4378,8 +5257,8 @@
     <mergeCell ref="A7:K7"/>
     <mergeCell ref="A8:K8"/>
     <mergeCell ref="A10:K10"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B17:F20"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B14:F20"/>
     <mergeCell ref="B21:F21"/>
     <mergeCell ref="B22:F25"/>
     <mergeCell ref="B26:F26"/>

</xml_diff>